<commit_message>
8 new files from Kate
</commit_message>
<xml_diff>
--- a/WorkplaceAnalytics/MyAnalytics/Use/MyA-Adoption/Norms-survey-questions.xlsx
+++ b/WorkplaceAnalytics/MyAnalytics/Use/MyA-Adoption/Norms-survey-questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanowak\OneDrive - Microsoft\MyA Customer Success\Docs docs\Drafts\Surveys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{40EEFE18-9029-4A7B-B02B-51D22AB583AF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{B001E78C-E876-48EE-813B-154C7797B6C1}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{40EEFE18-9029-4A7B-B02B-51D22AB583AF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{BC41FBFE-0847-4067-A7E3-313EB61F74E9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9348" xr2:uid="{13003A7A-E3E8-4B3E-AD07-7DF692C47D0F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
   <si>
     <t>We will carefully add essential recipients to our emails, not overuse the "Cc" field and transparently move people to "Bcc" when they are no longer needed on the thread.</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>We will aim to keep meetings as short as possible by scheduling meetings in 15-minute increments and carefully matching meeting duration with the agenda.</t>
+  </si>
+  <si>
+    <t>We will designate a "no meetings" day or period of time within a day, e.g. Friday afternoons, during which no meetings can be scheduled.</t>
   </si>
 </sst>
 </file>
@@ -504,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BC1F07-5F5C-458C-8998-C5024D6EBA70}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,7 +588,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -596,7 +599,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -607,7 +610,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -618,7 +621,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -629,7 +632,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -640,7 +643,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -651,7 +654,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -662,7 +665,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -673,7 +676,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -684,7 +687,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -695,10 +698,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
@@ -706,7 +709,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
@@ -717,7 +720,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
@@ -728,7 +731,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -739,7 +742,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
@@ -749,8 +752,8 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>25</v>
+      <c r="A22" t="s">
+        <v>2</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
@@ -760,8 +763,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>1</v>
+      <c r="A23" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
@@ -772,7 +775,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
         <v>29</v>
@@ -783,10 +786,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -794,7 +797,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -805,7 +808,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
@@ -816,12 +819,23 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
       <c r="C28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>